<commit_message>
bug fix in Eduati data files
</commit_message>
<xml_diff>
--- a/FALCON/ExampleDatasets/Eduati2017/CAR1_noCTRL_meas.xlsx
+++ b/FALCON/ExampleDatasets/Eduati2017/CAR1_noCTRL_meas.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebastien.delandtshe\Dropbox\Main\Eduati\DataFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\philippe.lucarelli\Documents\MATLAB\FALCON-dev\FALCON\ExampleDatasets\Eduati\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27285" windowHeight="15705" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27285" windowHeight="15705"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -430,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N87"/>
+  <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:N44"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="F61" sqref="F61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2372,221 +2372,6 @@
       </c>
       <c r="N44">
         <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A78">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87">
-        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -4549,7 +4334,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:N44"/>
     </sheetView>
   </sheetViews>

</xml_diff>